<commit_message>
Se agrega el campo de venta de alcohol en reporte de solicitudes
</commit_message>
<xml_diff>
--- a/static/docs/reporte_solicitudes.xlsx
+++ b/static/docs/reporte_solicitudes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\web\feria\static\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72C8DBBC-DD66-49BA-9223-E9064E844620}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC88C319-ED9C-4828-9D47-C1CB804ABCE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{7115F4C6-4B91-45CD-A163-19B41F0B5D19}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
   <si>
     <t>Folio de Solicitud</t>
   </si>
@@ -97,6 +97,9 @@
   </si>
   <si>
     <t>Descripción</t>
+  </si>
+  <si>
+    <t>Vende Alcohol</t>
   </si>
 </sst>
 </file>
@@ -178,7 +181,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -194,6 +197,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -533,7 +539,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7423B623-F707-4358-94CD-11A3F1679E26}">
-  <dimension ref="A1:X5653"/>
+  <dimension ref="A1:Y5653"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -548,39 +554,40 @@
     <col min="21" max="21" width="19.33203125" style="2" customWidth="1"/>
     <col min="22" max="22" width="29.77734375" style="2" customWidth="1"/>
     <col min="23" max="23" width="23" style="2" customWidth="1"/>
-    <col min="24" max="24" width="46.33203125" style="2" customWidth="1"/>
-    <col min="25" max="16384" width="11.5546875" style="2"/>
+    <col min="24" max="25" width="46.33203125" style="2" customWidth="1"/>
+    <col min="26" max="16384" width="11.5546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="44.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:25" ht="44.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
-      <c r="J1" s="7"/>
-      <c r="K1" s="7"/>
-      <c r="L1" s="7"/>
-      <c r="M1" s="7"/>
-      <c r="N1" s="7"/>
-      <c r="O1" s="7"/>
-      <c r="P1" s="7"/>
-      <c r="Q1" s="7"/>
-      <c r="R1" s="7"/>
-      <c r="S1" s="7"/>
-      <c r="T1" s="7"/>
-      <c r="U1" s="7"/>
-      <c r="V1" s="7"/>
-      <c r="W1" s="7"/>
-      <c r="X1" s="7"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
+      <c r="K1" s="8"/>
+      <c r="L1" s="8"/>
+      <c r="M1" s="8"/>
+      <c r="N1" s="8"/>
+      <c r="O1" s="8"/>
+      <c r="P1" s="8"/>
+      <c r="Q1" s="8"/>
+      <c r="R1" s="8"/>
+      <c r="S1" s="8"/>
+      <c r="T1" s="8"/>
+      <c r="U1" s="8"/>
+      <c r="V1" s="8"/>
+      <c r="W1" s="8"/>
+      <c r="X1" s="8"/>
+      <c r="Y1" s="7"/>
     </row>
-    <row r="2" spans="1:24" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:25" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -653,23 +660,26 @@
       <c r="X2" s="6" t="s">
         <v>23</v>
       </c>
+      <c r="Y2" s="6" t="s">
+        <v>24</v>
+      </c>
     </row>
-    <row r="3" spans="1:24" s="3" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3"/>
-    <row r="4" spans="1:24" s="3" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3"/>
-    <row r="5" spans="1:24" s="3" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3"/>
-    <row r="6" spans="1:24" s="3" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3"/>
-    <row r="7" spans="1:24" s="3" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3"/>
-    <row r="8" spans="1:24" s="3" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3"/>
-    <row r="9" spans="1:24" s="3" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3"/>
-    <row r="10" spans="1:24" s="3" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:25" s="3" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="1:25" s="3" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3"/>
+    <row r="5" spans="1:25" s="3" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3"/>
+    <row r="6" spans="1:25" s="3" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3"/>
+    <row r="7" spans="1:25" s="3" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3"/>
+    <row r="8" spans="1:25" s="3" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3"/>
+    <row r="9" spans="1:25" s="3" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3"/>
+    <row r="10" spans="1:25" s="3" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="J10" s="4"/>
     </row>
-    <row r="11" spans="1:24" s="3" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3"/>
-    <row r="12" spans="1:24" s="3" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3"/>
-    <row r="13" spans="1:24" s="3" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3"/>
-    <row r="14" spans="1:24" s="3" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3"/>
-    <row r="15" spans="1:24" s="3" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3"/>
-    <row r="16" spans="1:24" s="3" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3"/>
+    <row r="11" spans="1:25" s="3" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3"/>
+    <row r="12" spans="1:25" s="3" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3"/>
+    <row r="13" spans="1:25" s="3" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3"/>
+    <row r="14" spans="1:25" s="3" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3"/>
+    <row r="15" spans="1:25" s="3" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3"/>
+    <row r="16" spans="1:25" s="3" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3"/>
     <row r="17" s="3" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3"/>
     <row r="18" s="3" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3"/>
     <row r="19" s="3" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3"/>

</xml_diff>